<commit_message>
persistent counter and diff run data goes to diff sheets in csv
</commit_message>
<xml_diff>
--- a/face-directory/Output.xlsx
+++ b/face-directory/Output.xlsx
@@ -18,7 +18,313 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="346">
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
   <si>
     <t>combinedstore1</t>
   </si>
@@ -770,7 +1076,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="123">
+  <borders count="174">
     <border>
       <left/>
       <right/>
@@ -900,11 +1206,62 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1028,6 +1385,57 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="120" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="121" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="125" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,10 +1454,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>62</v>
+        <v>304</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2">
@@ -1057,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1065,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="0">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1073,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="0">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1081,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1089,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1107,10 +1515,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>142</v>
+        <v>344</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>143</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2">
@@ -1126,15 +1534,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1142,15 +1550,15 @@
         <v>0</v>
       </c>
       <c r="B5" s="0">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="0">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1184,26 +1592,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1211,21 +1619,23 @@
         <v>0</v>
       </c>
       <c r="B4" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
         <v>1</v>
       </c>
-      <c r="B5" s="0"/>
+      <c r="B5" s="0">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
         <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
appending data onto the same table
</commit_message>
<xml_diff>
--- a/face-directory/Output.xlsx
+++ b/face-directory/Output.xlsx
@@ -18,7 +18,271 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="434">
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
   <si>
     <t>combinedstore1</t>
   </si>
@@ -1076,7 +1340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="174">
+  <borders count="218">
     <border>
       <left/>
       <right/>
@@ -1257,11 +1521,55 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1436,6 +1744,50 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,18 +1806,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>304</v>
+        <v>432</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>305</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="0">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -1473,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="0">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -1481,15 +1833,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="0">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="0">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -1497,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
timing of mask + face presentation
</commit_message>
<xml_diff>
--- a/face-directory/Output.xlsx
+++ b/face-directory/Output.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,18 +10,48 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344698B2-0A6D-6040-BC81-32BD55A275E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
   <si>
     <t>combinedstore1</t>
   </si>
@@ -53,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -61,12 +91,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,47 +429,46 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="true"/>
+    <col min="2" max="2" width="15.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0"/>
+    </row>
+    <row r="3" x14ac:dyDescent="0.2">
+      <c r="A3" s="0">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.2">
+      <c r="A4" s="0">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.2">
+      <c r="A5" s="0">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="B5" s="0">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -441,16 +480,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="2" width="15.5" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -466,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -474,7 +513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -482,7 +521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
make mask more efficient
</commit_message>
<xml_diff>
--- a/face-directory/Output.xlsx
+++ b/face-directory/Output.xlsx
@@ -21,7 +21,529 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
   <si>
     <t>combinedstore1</t>
   </si>
@@ -83,7 +605,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="93">
     <border>
       <left/>
       <right/>
@@ -96,17 +618,191 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,24 +1131,26 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>186</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" s="0"/>
+      <c r="B2" s="0">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" s="0">
         <v>0</v>
       </c>
       <c r="B3" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
@@ -486,47 +1184,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" customWidth="true"/>
+    <col min="1" max="1" width="15.5703125" customWidth="true"/>
+    <col min="2" max="2" width="15.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0">
+        <v>9</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
+      <c r="A3" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="A4" s="0">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0">
+        <v>8</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
+      <c r="A5" s="0">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
counter fix (except not really)
</commit_message>
<xml_diff>
--- a/face-directory/Output.xlsx
+++ b/face-directory/Output.xlsx
@@ -15,13 +15,1046 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="532">
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
   <si>
     <t>combinedstore1</t>
   </si>
@@ -605,7 +1638,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="93">
+  <borders count="265">
     <border>
       <left/>
       <right/>
@@ -705,11 +1738,183 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -803,6 +2008,178 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="116" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="117" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="120" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="121" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="125" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="236" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="237" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="238" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="239" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="240" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="241" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="242" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="243" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="244" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="245" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="246" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="247" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="248" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="250" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="251" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,26 +2508,26 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="0" t="s">
-        <v>186</v>
+        <v>530</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>187</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="0">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
@@ -1158,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
@@ -1166,7 +2543,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1190,10 +2567,10 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="0" t="s">
-        <v>118</v>
+        <v>466</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>119</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
@@ -1201,7 +2578,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
@@ -1209,26 +2586,79 @@
         <v>0</v>
       </c>
       <c r="B3" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="0">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="true"/>
+    <col min="2" max="2" width="15.5703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make stats more clear and make boxplot
</commit_message>
<xml_diff>
--- a/face-directory/Output.xlsx
+++ b/face-directory/Output.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracypan/Documents/GitHub/tutorial-github-clps0950/midterm-project/face-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344698B2-0A6D-6040-BC81-32BD55A275E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A2EA88-5F30-454A-AC04-785B8F4AB881}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" fullCalcOnLoad="true"/>
@@ -22,691 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="532">
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
-  <si>
-    <t>combinedstore1</t>
-  </si>
-  <si>
-    <t>combinedstore2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="304">
   <si>
     <t>combinedstore1</t>
   </si>
@@ -1638,7 +954,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="265">
+  <borders count="152">
     <border>
       <left/>
       <right/>
@@ -1797,124 +1113,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -2067,119 +1270,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="236" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="237" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="238" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="239" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="240" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="241" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="242" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="243" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="244" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="245" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="246" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="247" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="248" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="249" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="250" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="251" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2496,65 +1586,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="true"/>
-    <col min="2" max="2" width="15.5703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
-        <v>0</v>
-      </c>
-      <c r="B4" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.2">
-      <c r="A5" s="0">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -2567,10 +1598,10 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="0" t="s">
-        <v>466</v>
+        <v>136</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>467</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
@@ -2578,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
@@ -2586,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
@@ -2594,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
@@ -2602,11 +1633,64 @@
         <v>1</v>
       </c>
       <c r="B5" s="0">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="true"/>
+    <col min="2" max="2" width="15.5703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
 
@@ -2621,15 +1705,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>504</v>
+        <v>302</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>505</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="0">
         <v>3</v>
@@ -2648,15 +1732,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small changes / comments
</commit_message>
<xml_diff>
--- a/face-directory/Output.xlsx
+++ b/face-directory/Output.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE76D32D-5558-C346-A85E-B05842FEA156}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+  <si>
+    <t>combinedstore1</t>
+  </si>
+  <si>
+    <t>combinedstore2</t>
+  </si>
   <si>
     <t>combinedstore1</t>
   </si>
@@ -74,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,13 +95,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,47 +426,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="true"/>
+    <col min="2" max="2" width="15.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
+    <row r="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+    <row r="2" x14ac:dyDescent="0.2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.2">
+      <c r="A3" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.2">
+      <c r="A4" s="0">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.2">
+      <c r="A5" s="0">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +485,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -492,7 +501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -500,7 +509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -508,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -531,7 +540,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -547,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -555,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -563,7 +572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -586,10 +595,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="2" width="15.5" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -597,7 +606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -605,7 +614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -613,7 +622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -621,7 +630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -638,16 +647,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="2" width="15.5" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -655,7 +664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -663,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -671,7 +680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -679,7 +688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -702,7 +711,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -718,7 +727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -726,7 +735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -734,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -757,7 +766,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -773,7 +782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -781,7 +790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -789,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -812,7 +821,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -828,7 +837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -836,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -844,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -867,7 +876,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -883,7 +892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -891,7 +900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -899,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -922,7 +931,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -938,7 +947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -946,7 +955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -954,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -977,7 +986,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1001,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1009,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>

</xml_diff>